<commit_message>
Calc prices of rides, filter data, check driver
Define price-function to be able to calc price of single ride
Filter data: Reduce data to rows which belong to specific month
Check if all active drivers are in table of drivers

Create python-dict from dictionary.xlsx
Set index of table of drivers
</commit_message>
<xml_diff>
--- a/data/logbook.xlsx
+++ b/data/logbook.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
   <si>
     <t xml:space="preserve">car</t>
   </si>
@@ -61,7 +61,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
+    <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
     <numFmt numFmtId="166" formatCode="HH:MM"/>
   </numFmts>
   <fonts count="5">
@@ -69,6 +69,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -90,6 +91,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -176,21 +178,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -216,7 +218,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>7</v>
       </c>
@@ -224,7 +226,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>36892</v>
+        <v>36891</v>
       </c>
       <c r="D2" s="2" t="n">
         <v>0.625</v>
@@ -241,22 +243,22 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>36893</v>
+        <v>36892</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>0.666666666666667</v>
+        <v>0.625</v>
       </c>
       <c r="E3" s="0" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F3" s="1" t="n">
-        <v>36893</v>
+        <v>36892</v>
       </c>
       <c r="G3" s="2" t="n">
         <v>0.708333333333333</v>
@@ -264,24 +266,70 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>36893</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>0.666666666666667</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>36893</v>
+      </c>
+      <c r="G4" s="2" t="n">
+        <v>0.708333333333333</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B5" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="1" t="n">
+      <c r="C5" s="1" t="n">
         <v>36896</v>
       </c>
-      <c r="D4" s="2" t="n">
+      <c r="D5" s="2" t="n">
         <v>0.0416666666666667</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E5" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>36896</v>
+      </c>
+      <c r="G5" s="2" t="n">
+        <v>0.541666666666667</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="1" t="n">
-        <v>36896</v>
-      </c>
-      <c r="G4" s="2" t="n">
+      <c r="C6" s="1" t="n">
+        <v>36923</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>36923</v>
+      </c>
+      <c r="G6" s="2" t="n">
         <v>0.541666666666667</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Use long car name
</commit_message>
<xml_diff>
--- a/data/logbook.xlsx
+++ b/data/logbook.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -43,13 +43,13 @@
     <t xml:space="preserve">timeEnd</t>
   </si>
   <si>
+    <t xml:space="preserve">AUR-UM192</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bert</t>
+  </si>
+  <si>
     <t xml:space="preserve">AurXX1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bert</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AurXX2</t>
   </si>
   <si>
     <t xml:space="preserve">Ernie</t>
@@ -181,18 +181,15 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7:G9"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="11.0714285714286"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -218,7 +215,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>7</v>
       </c>
@@ -243,7 +240,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>8</v>
@@ -266,7 +263,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>8</v>
@@ -289,7 +286,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>10</v>
@@ -312,7 +309,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>10</v>

</xml_diff>